<commit_message>
commit of streamlined plotting code
fixed scoping bug where summaries didn't work if there was a variable called response, updated the forest plots to use the existing summary functions, bug fixes
</commit_message>
<xml_diff>
--- a/data-raw/uvmodels.xlsx
+++ b/data-raw/uvmodels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lavery\OneDrive - UHN\Rpackages\reportRmd\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisaavery/Library/CloudStorage/OneDrive-UHN/Rpackages/reportRmd/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEE885CC-9CAE-484A-8A27-AACEFBC2FD7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79E7E05-19E0-FA47-A5A3-9AD0685E1D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="11340" xr2:uid="{688AD85A-7AF2-453B-BE2F-995267C440BC}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="16200" windowHeight="11340" xr2:uid="{688AD85A-7AF2-453B-BE2F-995267C440BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,13 +102,13 @@
     <t>rm_crr</t>
   </si>
   <si>
-    <t>rm_boxcos</t>
-  </si>
-  <si>
     <t>rm_gee</t>
   </si>
   <si>
     <t>raise_error</t>
+  </si>
+  <si>
+    <t>rm_boxcox</t>
   </si>
 </sst>
 </file>
@@ -164,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,7 +204,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -310,7 +310,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -452,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -463,15 +463,15 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -505,7 +505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -539,7 +539,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -553,7 +553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -567,7 +567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -578,13 +578,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -598,7 +598,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -612,7 +612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -623,13 +623,13 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -640,13 +640,13 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -657,13 +657,13 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -671,10 +671,10 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -682,10 +682,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -693,10 +693,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -704,10 +704,10 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -715,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>